<commit_message>
[CODE] actu config avec vraies features
</commit_message>
<xml_diff>
--- a/to_use/corps-features.xlsx
+++ b/to_use/corps-features.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\interface-Pascale\projet etudiants\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mes Documents\Polytech\INFO 4\Projet Transversal\algolov\to_use\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,9 +15,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$61</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="127">
   <si>
     <t>features_FR</t>
   </si>
@@ -402,12 +402,18 @@
   </si>
   <si>
     <t>En parlant de toi. Quelles sont les caractéristiques corporelles importantes pour te décrire?</t>
+  </si>
+  <si>
+    <t>Ajouté</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -772,101 +778,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.140625" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.28515625" customWidth="1"/>
-    <col min="5" max="6" width="34.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="65.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="65.28515625" customWidth="1"/>
+    <col min="6" max="7" width="34.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -874,61 +887,68 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="1">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="H6" t="s">
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="I6" t="s">
         <v>122</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D7" s="1">
-        <v>2</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="H7" t="s">
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="I7" t="s">
         <v>104</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -936,23 +956,26 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D9" s="1">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="H9" t="s">
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="I9" t="s">
         <v>124</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -960,17 +983,20 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="1">
-        <v>2</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -978,17 +1004,20 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="1">
-        <v>2</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E11" s="1">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -996,17 +1025,20 @@
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="1">
-        <v>2</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1014,17 +1046,20 @@
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="1">
-        <v>2</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E13" s="1">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1032,34 +1067,40 @@
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="1">
-        <v>2</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E14" s="1">
+        <v>2</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D15" s="1">
-        <v>2</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E15" s="1">
+        <v>2</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1067,17 +1108,20 @@
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="1">
-        <v>2</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1085,17 +1129,20 @@
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="1">
-        <v>2</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E17" s="1">
+        <v>2</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1103,17 +1150,20 @@
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="1">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="E18" s="1">
+        <v>2</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:7" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1121,45 +1171,50 @@
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="1">
-        <v>2</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="1">
+        <v>2</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1167,16 +1222,19 @@
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D22" s="1">
-        <v>2</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E22" s="1">
+        <v>2</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1184,92 +1242,102 @@
         <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="1">
-        <v>2</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="1:6" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="1">
+        <v>2</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="6">
         <v>0</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="6"/>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F24" s="1"/>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D25" s="1">
-        <v>2</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="1">
+        <v>2</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="1"/>
+      <c r="D26" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-    </row>
-    <row r="27" spans="1:6" ht="75.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" ht="150.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="1"/>
+      <c r="D27" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="4"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="4"/>
+      <c r="G27" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1277,17 +1345,20 @@
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D29" s="1">
-        <v>2</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E29" s="1">
+        <v>2</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -1295,17 +1366,20 @@
         <v>1</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="1">
-        <v>2</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E30" s="1">
+        <v>2</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -1313,17 +1387,20 @@
         <v>1</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D31" s="1">
-        <v>2</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E31" s="1">
+        <v>2</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -1331,31 +1408,35 @@
         <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D32" s="1">
-        <v>2</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E32" s="1">
+        <v>2</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B33" s="2">
         <v>0</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2"/>
+      <c r="D33" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
@@ -1363,17 +1444,20 @@
         <v>1</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D34" s="1">
-        <v>2</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E34" s="1">
+        <v>2</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -1381,17 +1465,20 @@
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D35" s="1">
-        <v>2</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E35" s="1">
+        <v>2</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
@@ -1399,67 +1486,77 @@
         <v>1</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D36" s="1">
-        <v>2</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E36" s="1">
+        <v>2</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B37" s="1">
         <v>1</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="1">
-        <v>2</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="E37" s="1">
+        <v>2</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B38" s="1">
         <v>1</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D38" s="1">
-        <v>2</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F38" s="5"/>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E38" s="1">
+        <v>2</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="4">
         <v>0</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="4"/>
+      <c r="D39" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -1467,17 +1564,20 @@
         <v>1</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D40" s="1">
-        <v>2</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="1:6" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="E40" s="1">
+        <v>2</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -1485,95 +1585,105 @@
         <v>1</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D41" s="1">
-        <v>2</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E41" s="1">
+        <v>2</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B42" s="1">
         <v>0</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="1"/>
+      <c r="D42" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B43" s="1">
         <v>0</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="1"/>
+      <c r="D43" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="5">
         <v>1</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D44" s="1">
-        <v>2</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E44" s="1">
+        <v>2</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B45" s="1">
         <v>0</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="1"/>
+      <c r="D45" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B46" s="1">
         <v>0</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="1"/>
+      <c r="D46" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D46" s="1">
-        <v>2</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E46" s="1">
+        <v>2</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
@@ -1581,71 +1691,79 @@
         <v>1</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D47" s="1">
-        <v>2</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E47" s="1">
+        <v>2</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B48" s="1">
         <v>1</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="1"/>
+      <c r="D48" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D48" s="1">
-        <v>2</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E48" s="1">
+        <v>2</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B49" s="1">
         <v>1</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="1"/>
+      <c r="D49" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D49" s="1">
-        <v>2</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F49" s="1"/>
-    </row>
-    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E49" s="1">
+        <v>2</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B50" s="1">
         <v>1</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C50" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D50" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D50" s="1">
-        <v>2</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F50" s="1"/>
-    </row>
-    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E50" s="1">
+        <v>2</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
@@ -1653,17 +1771,20 @@
         <v>1</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D51" s="1">
-        <v>2</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F51" s="1"/>
-    </row>
-    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E51" s="1">
+        <v>2</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
@@ -1671,17 +1792,20 @@
         <v>1</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D52" s="1">
-        <v>2</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E52" s="1">
+        <v>2</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
@@ -1689,17 +1813,20 @@
         <v>1</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D53" s="1">
-        <v>2</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="1:6" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="E53" s="1">
+        <v>2</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="1:7" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
@@ -1707,34 +1834,38 @@
         <v>1</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D54" s="1">
-        <v>2</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F54" s="4"/>
-    </row>
-    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E54" s="1">
+        <v>2</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G54" s="4"/>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B55" s="1">
         <v>1</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="1"/>
+      <c r="D55" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D55" s="1">
-        <v>2</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E55" s="1">
+        <v>2</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
@@ -1742,16 +1873,19 @@
         <v>1</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D56" s="1">
-        <v>2</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E56" s="1">
+        <v>2</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
@@ -1759,29 +1893,33 @@
         <v>1</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="1">
-        <v>2</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="60.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E57" s="1">
+        <v>2</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B58" s="1">
         <v>0</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="1"/>
+      <c r="D58" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D58" s="1"/>
       <c r="E58" s="1"/>
-    </row>
-    <row r="59" spans="1:6" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="1:7" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
@@ -1789,16 +1927,19 @@
         <v>1</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D59" s="1">
-        <v>2</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E59" s="1">
+        <v>2</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
@@ -1806,16 +1947,19 @@
         <v>1</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D60" s="1">
-        <v>2</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E60" s="1">
+        <v>2</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>60</v>
       </c>
@@ -1823,23 +1967,20 @@
         <v>1</v>
       </c>
       <c r="C61" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D61" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D61" s="1">
-        <v>2</v>
-      </c>
-      <c r="E61" s="1" t="s">
+      <c r="E61" s="1">
+        <v>2</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>107</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G61">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H61"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>